<commit_message>
fix label on A150 (74.4 to 74.3 for piaB)
</commit_message>
<xml_diff>
--- a/Data/cleaned/A150_scope_2021_05_24_DC.xlsx
+++ b/Data/cleaned/A150_scope_2021_05_24_DC.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ay327\Desktop\SMpfizer\SCOPE applied DC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DMW63\Desktop\R_Projects\scope_qpcr_analysis\Data\cleaned\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4FBA536-949B-4C60-B3D0-0C173B7341C0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2FB3FE3-5B4A-494F-9F88-9C1730B6DBFD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="A150_scope_2021_05_24" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="184">
   <si>
     <t>File Name</t>
   </si>
@@ -358,9 +358,6 @@
     <t>D02</t>
   </si>
   <si>
-    <t>12.3</t>
-  </si>
-  <si>
     <t>D03</t>
   </si>
   <si>
@@ -427,9 +424,6 @@
     <t>E01</t>
   </si>
   <si>
-    <t>74.4</t>
-  </si>
-  <si>
     <t>piaB</t>
   </si>
   <si>
@@ -575,6 +569,9 @@
   </si>
   <si>
     <t>H12</t>
+  </si>
+  <si>
+    <t>12.4</t>
   </si>
 </sst>
 </file>
@@ -647,7 +644,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
       <protection locked="0"/>
@@ -675,6 +672,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -993,11 +993,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="K111" sqref="K111"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E70" sqref="E70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" style="2" customWidth="1"/>
     <col min="2" max="2" width="10" style="3" customWidth="1"/>
@@ -1009,7 +1009,7 @@
     <col min="9" max="16384" width="10" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1017,7 +1017,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1025,18 +1025,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="4"/>
     </row>
-    <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -1044,7 +1044,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -1052,7 +1052,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -1060,7 +1060,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -1068,7 +1068,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -1076,7 +1076,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
@@ -1084,7 +1084,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -1092,7 +1092,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>18</v>
       </c>
@@ -1100,7 +1100,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>20</v>
       </c>
@@ -1108,7 +1108,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>22</v>
       </c>
@@ -1116,7 +1116,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>24</v>
       </c>
@@ -1124,12 +1124,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>26</v>
       </c>
@@ -1152,7 +1152,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>33</v>
       </c>
@@ -1175,7 +1175,7 @@
         <v>37.037460447796697</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>39</v>
       </c>
@@ -1198,7 +1198,7 @@
         <v>26.842248627671399</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>41</v>
       </c>
@@ -1221,7 +1221,7 @@
         <v>37.166226273137703</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>43</v>
       </c>
@@ -1241,7 +1241,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>45</v>
       </c>
@@ -1261,7 +1261,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>47</v>
       </c>
@@ -1284,7 +1284,7 @@
         <v>25.7941220541551</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>49</v>
       </c>
@@ -1304,7 +1304,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>51</v>
       </c>
@@ -1324,7 +1324,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>53</v>
       </c>
@@ -1344,7 +1344,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>55</v>
       </c>
@@ -1364,7 +1364,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>57</v>
       </c>
@@ -1384,7 +1384,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>59</v>
       </c>
@@ -1404,7 +1404,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>61</v>
       </c>
@@ -1424,7 +1424,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>63</v>
       </c>
@@ -1444,7 +1444,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>65</v>
       </c>
@@ -1464,7 +1464,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>67</v>
       </c>
@@ -1484,7 +1484,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>69</v>
       </c>
@@ -1504,7 +1504,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>71</v>
       </c>
@@ -1524,7 +1524,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>73</v>
       </c>
@@ -1547,7 +1547,7 @@
         <v>26.971919612800299</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>75</v>
       </c>
@@ -1567,7 +1567,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>77</v>
       </c>
@@ -1587,7 +1587,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>79</v>
       </c>
@@ -1607,7 +1607,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>81</v>
       </c>
@@ -1627,7 +1627,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>83</v>
       </c>
@@ -1647,7 +1647,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>85</v>
       </c>
@@ -1667,7 +1667,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>87</v>
       </c>
@@ -1687,7 +1687,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>89</v>
       </c>
@@ -1707,7 +1707,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>91</v>
       </c>
@@ -1727,7 +1727,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>93</v>
       </c>
@@ -1747,7 +1747,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>95</v>
       </c>
@@ -1767,7 +1767,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>97</v>
       </c>
@@ -1790,7 +1790,7 @@
         <v>21.652628358986998</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>99</v>
       </c>
@@ -1813,7 +1813,7 @@
         <v>24.104078454439598</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>101</v>
       </c>
@@ -1833,7 +1833,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>103</v>
       </c>
@@ -1853,7 +1853,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>105</v>
       </c>
@@ -1873,7 +1873,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>107</v>
       </c>
@@ -1893,7 +1893,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>109</v>
       </c>
@@ -1916,7 +1916,7 @@
         <v>24.591404084243301</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>111</v>
       </c>
@@ -1929,128 +1929,128 @@
       <c r="D58" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="E58" s="7" t="s">
+      <c r="E58" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="F58" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="F58" s="7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A59" s="2" t="s">
+      <c r="B59" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C59" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D59" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E59" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="B59" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C59" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D59" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E59" s="7" t="s">
+      <c r="F59" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="F59" s="7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A60" s="2" t="s">
+      <c r="B60" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C60" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D60" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E60" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="B60" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C60" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D60" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E60" s="7" t="s">
+      <c r="F60" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F60" s="7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A61" s="2" t="s">
+      <c r="B61" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C61" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D61" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E61" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="B61" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C61" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D61" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E61" s="7" t="s">
+      <c r="F61" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="F61" s="7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A62" s="2" t="s">
+      <c r="B62" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C62" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D62" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E62" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="B62" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C62" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D62" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E62" s="7" t="s">
+      <c r="F62" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="F62" s="7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A63" s="2" t="s">
+      <c r="B63" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C63" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D63" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="B63" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C63" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D63" s="7" t="s">
+      <c r="E63" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F63" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="E63" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="F63" s="7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A64" s="2" t="s">
+      <c r="B64" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C64" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D64" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="B64" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C64" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D64" s="7" t="s">
+      <c r="E64" s="7" t="s">
         <v>124</v>
-      </c>
-      <c r="E64" s="7" t="s">
-        <v>125</v>
       </c>
       <c r="F64" s="7" t="s">
         <v>38</v>
@@ -2059,21 +2059,21 @@
         <v>23.435581095217</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C65" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D65" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="E65" s="7" t="s">
         <v>126</v>
-      </c>
-      <c r="B65" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C65" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D65" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="E65" s="7" t="s">
-        <v>127</v>
       </c>
       <c r="F65" s="7" t="s">
         <v>38</v>
@@ -2082,21 +2082,21 @@
         <v>26.907441200782198</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C66" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D66" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="E66" s="7" t="s">
         <v>128</v>
-      </c>
-      <c r="B66" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C66" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D66" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="E66" s="7" t="s">
-        <v>129</v>
       </c>
       <c r="F66" s="7" t="s">
         <v>38</v>
@@ -2105,21 +2105,21 @@
         <v>30.492725771827601</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C67" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D67" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="E67" s="7" t="s">
         <v>130</v>
-      </c>
-      <c r="B67" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C67" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D67" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="E67" s="7" t="s">
-        <v>131</v>
       </c>
       <c r="F67" s="7" t="s">
         <v>38</v>
@@ -2128,21 +2128,21 @@
         <v>34.8725772649193</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C68" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D68" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="E68" s="7" t="s">
         <v>132</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C68" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D68" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="E68" s="7" t="s">
-        <v>133</v>
       </c>
       <c r="F68" s="7" t="s">
         <v>38</v>
@@ -2151,9 +2151,9 @@
         <v>41.384131837448301</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>34</v>
@@ -2164,16 +2164,16 @@
       <c r="D69" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="E69" s="7" t="s">
+      <c r="E69" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="F69" s="7" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="2" t="s">
         <v>135</v>
-      </c>
-      <c r="F69" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A70" s="2" t="s">
-        <v>137</v>
       </c>
       <c r="B70" s="3" t="s">
         <v>34</v>
@@ -2188,12 +2188,12 @@
         <v>40</v>
       </c>
       <c r="F70" s="7" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="2" t="s">
         <v>136</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A71" s="2" t="s">
-        <v>138</v>
       </c>
       <c r="B71" s="3" t="s">
         <v>34</v>
@@ -2208,12 +2208,12 @@
         <v>42</v>
       </c>
       <c r="F71" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B72" s="3" t="s">
         <v>34</v>
@@ -2228,15 +2228,15 @@
         <v>44</v>
       </c>
       <c r="F72" s="7" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G72" s="8">
         <v>38.217401141292598</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B73" s="3" t="s">
         <v>34</v>
@@ -2251,12 +2251,12 @@
         <v>46</v>
       </c>
       <c r="F73" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B74" s="3" t="s">
         <v>34</v>
@@ -2271,15 +2271,15 @@
         <v>48</v>
       </c>
       <c r="F74" s="7" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G74" s="8">
         <v>32.454004445647001</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B75" s="3" t="s">
         <v>34</v>
@@ -2294,12 +2294,12 @@
         <v>50</v>
       </c>
       <c r="F75" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B76" s="3" t="s">
         <v>34</v>
@@ -2314,12 +2314,12 @@
         <v>52</v>
       </c>
       <c r="F76" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B77" s="3" t="s">
         <v>34</v>
@@ -2334,12 +2334,12 @@
         <v>54</v>
       </c>
       <c r="F77" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B78" s="3" t="s">
         <v>34</v>
@@ -2354,12 +2354,12 @@
         <v>56</v>
       </c>
       <c r="F78" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B79" s="3" t="s">
         <v>34</v>
@@ -2374,12 +2374,12 @@
         <v>58</v>
       </c>
       <c r="F79" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B80" s="3" t="s">
         <v>34</v>
@@ -2394,12 +2394,12 @@
         <v>60</v>
       </c>
       <c r="F80" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B81" s="3" t="s">
         <v>34</v>
@@ -2414,12 +2414,12 @@
         <v>62</v>
       </c>
       <c r="F81" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B82" s="3" t="s">
         <v>34</v>
@@ -2434,12 +2434,12 @@
         <v>64</v>
       </c>
       <c r="F82" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B83" s="3" t="s">
         <v>34</v>
@@ -2454,12 +2454,12 @@
         <v>66</v>
       </c>
       <c r="F83" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B84" s="3" t="s">
         <v>34</v>
@@ -2474,12 +2474,12 @@
         <v>68</v>
       </c>
       <c r="F84" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B85" s="3" t="s">
         <v>34</v>
@@ -2494,12 +2494,12 @@
         <v>70</v>
       </c>
       <c r="F85" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B86" s="3" t="s">
         <v>34</v>
@@ -2514,12 +2514,12 @@
         <v>72</v>
       </c>
       <c r="F86" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B87" s="3" t="s">
         <v>34</v>
@@ -2534,12 +2534,12 @@
         <v>74</v>
       </c>
       <c r="F87" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B88" s="3" t="s">
         <v>34</v>
@@ -2554,12 +2554,12 @@
         <v>76</v>
       </c>
       <c r="F88" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B89" s="3" t="s">
         <v>34</v>
@@ -2574,12 +2574,12 @@
         <v>78</v>
       </c>
       <c r="F89" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B90" s="3" t="s">
         <v>34</v>
@@ -2594,12 +2594,12 @@
         <v>80</v>
       </c>
       <c r="F90" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B91" s="3" t="s">
         <v>34</v>
@@ -2614,12 +2614,12 @@
         <v>82</v>
       </c>
       <c r="F91" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B92" s="3" t="s">
         <v>34</v>
@@ -2634,12 +2634,12 @@
         <v>84</v>
       </c>
       <c r="F92" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B93" s="3" t="s">
         <v>34</v>
@@ -2654,12 +2654,12 @@
         <v>86</v>
       </c>
       <c r="F93" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B94" s="3" t="s">
         <v>34</v>
@@ -2674,12 +2674,12 @@
         <v>88</v>
       </c>
       <c r="F94" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B95" s="3" t="s">
         <v>34</v>
@@ -2694,12 +2694,12 @@
         <v>90</v>
       </c>
       <c r="F95" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B96" s="3" t="s">
         <v>34</v>
@@ -2714,12 +2714,12 @@
         <v>92</v>
       </c>
       <c r="F96" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B97" s="3" t="s">
         <v>34</v>
@@ -2734,15 +2734,15 @@
         <v>94</v>
       </c>
       <c r="F97" s="7" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G97" s="8">
         <v>33.280035547205301</v>
       </c>
     </row>
-    <row r="98" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="98" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B98" s="3" t="s">
         <v>34</v>
@@ -2757,12 +2757,12 @@
         <v>96</v>
       </c>
       <c r="F98" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B99" s="3" t="s">
         <v>34</v>
@@ -2777,12 +2777,12 @@
         <v>98</v>
       </c>
       <c r="F99" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="100" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B100" s="3" t="s">
         <v>34</v>
@@ -2797,12 +2797,12 @@
         <v>100</v>
       </c>
       <c r="F100" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B101" s="3" t="s">
         <v>34</v>
@@ -2817,12 +2817,12 @@
         <v>102</v>
       </c>
       <c r="F101" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="102" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B102" s="3" t="s">
         <v>34</v>
@@ -2837,12 +2837,12 @@
         <v>104</v>
       </c>
       <c r="F102" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="103" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B103" s="3" t="s">
         <v>34</v>
@@ -2857,32 +2857,32 @@
         <v>106</v>
       </c>
       <c r="F103" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C104" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D104" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E104" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="F104" s="7" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="2" t="s">
         <v>171</v>
-      </c>
-      <c r="B104" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C104" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D104" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E104" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="F104" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="105" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A105" s="2" t="s">
-        <v>173</v>
       </c>
       <c r="B105" s="3" t="s">
         <v>34</v>
@@ -2897,133 +2897,133 @@
         <v>110</v>
       </c>
       <c r="F105" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="106" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B106" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C106" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D106" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E106" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="F106" s="7" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="B107" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C107" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D107" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E107" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="F107" s="7" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="B106" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C106" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D106" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E106" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F106" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A107" s="2" t="s">
+      <c r="B108" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C108" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D108" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E108" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="F108" s="7" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="B107" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C107" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D107" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E107" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="F107" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="108" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A108" s="2" t="s">
+      <c r="B109" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C109" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D109" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E109" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="F109" s="7" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="B108" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C108" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D108" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E108" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="F108" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="109" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A109" s="2" t="s">
+      <c r="B110" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C110" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D110" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E110" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="F110" s="7" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="B109" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C109" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D109" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E109" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="F109" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="110" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A110" s="2" t="s">
+      <c r="B111" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C111" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D111" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="E111" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F111" s="7" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="B110" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C110" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D110" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E110" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="F110" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="111" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A111" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="B111" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C111" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D111" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="E111" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="F111" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="112" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A112" s="2" t="s">
-        <v>180</v>
-      </c>
       <c r="B112" s="3" t="s">
         <v>34</v>
       </c>
@@ -3031,21 +3031,21 @@
         <v>35</v>
       </c>
       <c r="D112" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="E112" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="E112" s="7" t="s">
-        <v>125</v>
-      </c>
       <c r="F112" s="7" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G112" s="8">
         <v>22.0428135513847</v>
       </c>
     </row>
-    <row r="113" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="113" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B113" s="3" t="s">
         <v>34</v>
@@ -3054,21 +3054,21 @@
         <v>35</v>
       </c>
       <c r="D113" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E113" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F113" s="7" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G113" s="8">
         <v>25.813423148259599</v>
       </c>
     </row>
-    <row r="114" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="114" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B114" s="3" t="s">
         <v>34</v>
@@ -3077,21 +3077,21 @@
         <v>35</v>
       </c>
       <c r="D114" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E114" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F114" s="7" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G114" s="8">
         <v>29.160400687859202</v>
       </c>
     </row>
-    <row r="115" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="115" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B115" s="3" t="s">
         <v>34</v>
@@ -3100,21 +3100,21 @@
         <v>35</v>
       </c>
       <c r="D115" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E115" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F115" s="7" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G115" s="8">
         <v>34.375753936707902</v>
       </c>
     </row>
-    <row r="116" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="116" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B116" s="3" t="s">
         <v>34</v>
@@ -3123,13 +3123,13 @@
         <v>35</v>
       </c>
       <c r="D116" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E116" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F116" s="7" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>

</xml_diff>